<commit_message>
fix bug order export
</commit_message>
<xml_diff>
--- a/TeduShop.WebAPI/Templates/OrderTemplate.xlsx
+++ b/TeduShop.WebAPI/Templates/OrderTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoct\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\tedushop-webapi\TeduShop.WebAPI\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>HÓA ĐƠN BÁN HÀNG</t>
   </si>
@@ -50,19 +50,6 @@
     <t>TỔNG CỘNG</t>
   </si>
   <si>
-    <r>
-      <t>Thành tiền (viết bằng chữ):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> ............................................................................................................................
-....................................................................................................................................................................</t>
-    </r>
-  </si>
-  <si>
     <t>Ngày ......... tháng ......... năm 20.........</t>
   </si>
   <si>
@@ -70,9 +57,6 @@
   </si>
   <si>
     <t>NGƯỜI BÁN HÀNG</t>
-  </si>
-  <si>
-    <t>TEDU SHOP</t>
   </si>
   <si>
     <t>Địa chỉ: Xuân La Tây Hồ Hà Nội
@@ -82,13 +66,10 @@
     <t>Mặt hàng bán (Thời trang nam)</t>
   </si>
   <si>
-    <t>SĐT</t>
-  </si>
-  <si>
-    <t>0966 036 626</t>
-  </si>
-  <si>
     <t>Điện thoại:</t>
+  </si>
+  <si>
+    <t>SĐT: 0966 026 626</t>
   </si>
 </sst>
 </file>
@@ -220,7 +201,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -269,11 +250,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -281,38 +280,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -330,6 +308,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1619251</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>828676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1181100" y="19050"/>
+          <a:ext cx="809626" cy="809626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,7 +625,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -610,62 +637,58 @@
     <col min="5" max="5" width="19.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="B3" s="29"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+        <v>14</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -865,10 +888,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="3">
         <f>SUM(C9:C23)</f>
         <v>0</v>
@@ -879,50 +902,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+    <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="25"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C28" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C28" s="22" t="s">
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.55069444444444449" right="0.2361111111111111" top="0.47222222222222221" bottom="0.35416666666666669" header="0.31458333333333333" footer="0.27500000000000002"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>